<commit_message>
Implementación impresión a cheque según plantilla
</commit_message>
<xml_diff>
--- a/ChequesPamacri/src/TmpCheque.xlsx
+++ b/ChequesPamacri/src/TmpCheque.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Documents\NetBeansProjects\ChequesPamacri\ChequesPamacri\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elxpa\Documents\NetBeansProjects\ChequesPamacri\ChequesPamacri\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72F53BF-6CB2-43CE-AC6A-779DFEF574E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6146258-05CB-4263-A3F5-164FF5167C99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0414D509-7EA4-40E1-A67F-86D77AEABF9D}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11505" xr2:uid="{0414D509-7EA4-40E1-A67F-86D77AEABF9D}"/>
   </bookViews>
   <sheets>
     <sheet name="CHEQUE" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -44,41 +44,40 @@
     <t>STGO</t>
   </si>
   <si>
-    <t>año</t>
+    <t>RODRIGO FAZEKAS VARGAS</t>
   </si>
   <si>
-    <t>mes</t>
+    <t>SETENTA Y OCHO MILLONES QUINIENTOS NOVENTA Y OCHO MIL SETECIENTOS CUARENTA Y UN PESOS</t>
   </si>
   <si>
-    <t>dia</t>
+    <t>ALIMENTOS FRUNA LIMITADA</t>
   </si>
   <si>
-    <t>monto total del cheque</t>
+    <t>CUARENTA Y OCHO MILLONES QUINIENTOS SETENTA Y OCHO MIL CIENTO DOCE PESOS</t>
   </si>
   <si>
-    <t>monto del cheque escrito</t>
+    <t>BODEGAS Y VINEDOS DE AGUIRRE S.A.</t>
   </si>
   <si>
-    <t>nombre destino</t>
+    <t>CUATROCIENTOS TREINTA Y DOS MILLONES QUINIENTOS TREINTA Y DOS MIL CUATROCIENTOS CINCUENTA Y TRES PESOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="\ \ \ \ \ \ \ \ \ #\ \ #\ \ #\ \ #\ \ #\ \ \ #\ \ \ #\ \ \ #\ \ \ 0"/>
     <numFmt numFmtId="165" formatCode="#\ #\ #\ #\ #\ #\ #\ #\ 0"/>
-    <numFmt numFmtId="166" formatCode="#\ \ \ \ #"/>
-    <numFmt numFmtId="167" formatCode="#\ \ #"/>
-    <numFmt numFmtId="168" formatCode="\ #\ #"/>
-    <numFmt numFmtId="169" formatCode="\ #\ #\ #\ #\ \ "/>
-    <numFmt numFmtId="170" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="&quot;$&quot;\ #,##0"/>
-    <numFmt numFmtId="172" formatCode="#&quot;.&quot;###&quot;.&quot;###&quot;-&quot;#\ "/>
-    <numFmt numFmtId="173" formatCode="#,##0&quot;.-&quot;"/>
+    <numFmt numFmtId="166" formatCode="#\ \ #"/>
+    <numFmt numFmtId="167" formatCode="\ #\ #"/>
+    <numFmt numFmtId="168" formatCode="\ #\ #\ #\ #\ \ "/>
+    <numFmt numFmtId="169" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="171" formatCode="#&quot;.&quot;###&quot;.&quot;###&quot;-&quot;#\ "/>
+    <numFmt numFmtId="172" formatCode="#,##0&quot;.-&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,27 +109,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Berlin Sans FB"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Berlin Sans FB"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.8"/>
-      <color theme="1"/>
-      <name val="Berlin Sans FB"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="CMC7"/>
@@ -142,6 +120,12 @@
       <color theme="1"/>
       <name val="CMC7"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Berlin Sans FB"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,9 +151,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment vertical="center"/>
@@ -183,52 +167,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -903,54 +890,54 @@
   <dimension ref="B1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="1.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="1.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="1" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="2.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="1.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="1.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="4.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="4.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="2.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="5.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="1.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="1.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="2.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" hidden="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="16" max="16384" style="1" width="11.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="38.25" customHeight="1"/>
     <row r="2" spans="2:16" ht="5.25" customHeight="1">
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
     </row>
     <row r="3" spans="2:16" ht="15" customHeight="1">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="F3" s="16" t="s">
-        <v>4</v>
+      <c r="F3" s="15" t="n">
+        <v>4.32532453E8</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="2:16" ht="8.4499999999999993" customHeight="1">
       <c r="B4" s="2"/>
@@ -968,75 +955,76 @@
     <row r="5" spans="2:16" ht="19.7" customHeight="1">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
-        <v>3</v>
+      <c r="I5" s="20" t="n">
+        <v>15.0</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9" t="s">
+      <c r="J5" s="5">
         <v>1</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="11">
-        <f>MONTH([1]ingreso!B8)</f>
+      <c r="K5" s="21" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="22" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="8">
         <v>1</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" ht="25.5" customHeight="1">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>6</v>
+      <c r="D6" s="17" t="s">
+        <v>5</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" spans="2:16" ht="19.5" customHeight="1">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="20" t="s">
-        <v>5</v>
+      <c r="D7" s="19" t="s">
+        <v>6</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="P7" s="13"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="12"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="2:16" ht="10.5" customHeight="1">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="2:16">
       <c r="B9" s="2"/>
@@ -1047,20 +1035,20 @@
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="2:16" ht="15" customHeight="1">
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="2:16" ht="21" customHeight="1">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="I12" s="21" t="str">
+      <c r="I12" s="13" t="n">
         <f>F3</f>
-        <v>monto total del cheque</v>
+        <v>4.32532453E8</v>
       </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="2:16" ht="18" customHeight="1"/>
   </sheetData>
@@ -1070,7 +1058,7 @@
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D6:M6"/>
-    <mergeCell ref="D7:M8"/>
+    <mergeCell ref="D7:L8"/>
   </mergeCells>
   <pageMargins left="1.4173228346456694" right="0.19685039370078741" top="0.15748031496062992" bottom="0.23622047244094491" header="0.23622047244094491" footer="0.74803149606299213"/>
   <pageSetup paperSize="74" fitToWidth="0" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>